<commit_message>
Ajout des tâches dans la répartition des tâches
</commit_message>
<xml_diff>
--- a/Documents/repartition_des_taches.xlsx
+++ b/Documents/repartition_des_taches.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Répartition des tâches</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t>Loueslati Taoufik</t>
+  </si>
+  <si>
+    <t>Client/appli android</t>
+  </si>
+  <si>
+    <t>Serveur/raspberry pi</t>
+  </si>
+  <si>
+    <t>Serveur : Envoie de la vidéo</t>
+  </si>
+  <si>
+    <t>Client : réception/affichage de la vidéo</t>
+  </si>
+  <si>
+    <t>Client : commande des roues</t>
   </si>
 </sst>
 </file>
@@ -91,10 +106,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,31 +393,53 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="36.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">

</xml_diff>